<commit_message>
Exercise 13.2 and 13.3 working on STM32VL
</commit_message>
<xml_diff>
--- a/Exercise13p3-Interrupt_Triggered_DAC/stm32 timer worksheet.xlsx
+++ b/Exercise13p3-Interrupt_Triggered_DAC/stm32 timer worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\OneDrive\Documents\DiscoveringSTM32\Exercise13p3-Interrupt_Triggered_DAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2662034-9FAE-40C5-AFB3-71497A2C3B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5748F9A7-99A1-41A5-A0A4-E887D601D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B03197A-48E6-4BCF-AE5C-62A4470EC6D8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Syscoreclk</t>
   </si>
@@ -91,16 +91,20 @@
   </si>
   <si>
     <t>~44.1kHz - close enough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44100 Delta </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +114,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,18 +145,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C80083-E709-4F3B-8838-F172476268C3}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
@@ -594,7 +609,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -602,31 +617,31 @@
       <c r="A6" s="1">
         <v>24000000</v>
       </c>
-      <c r="B6" s="2">
-        <v>18000000</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
+      <c r="B6" s="6">
+        <v>4000000</v>
+      </c>
+      <c r="C6" s="7">
+        <f>A6/B6</f>
+        <v>6</v>
       </c>
       <c r="D6">
         <f>A6/C6</f>
-        <v>6000000</v>
+        <v>4000000</v>
       </c>
       <c r="E6" s="3">
         <f>1/D6</f>
-        <v>1.6666666666666668E-7</v>
+        <v>2.4999999999999999E-7</v>
       </c>
       <c r="F6">
-        <f>408/3</f>
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="G6">
         <f>D6/F6</f>
-        <v>44117.647058823532</v>
+        <v>43956.043956043955</v>
       </c>
       <c r="H6">
         <f>1/G6</f>
-        <v>2.2666666666666664E-5</v>
+        <v>2.2750000000000001E-5</v>
       </c>
       <c r="J6" s="4"/>
       <c r="L6" t="s">
@@ -637,6 +652,13 @@
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
+      <c r="F7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <f>44100-G6</f>
+        <v>143.9560439560446</v>
+      </c>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -703,12 +725,6 @@
       <c r="F10">
         <f>D10/E10</f>
         <v>179972100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <f>72000000/4</f>
-        <v>18000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>